<commit_message>
FE Cosmetics fix on Polesite table
</commit_message>
<xml_diff>
--- a/website/backend/model/polesites/test/Alsace Bonnet Sungau 09-03.xlsx
+++ b/website/backend/model/polesites/test/Alsace Bonnet Sungau 09-03.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294C74B3-276F-46E3-AFC2-D9F29A0DCA59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DE152F-12F0-4508-903C-DC2C8B30F375}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="5745" windowWidth="47595" windowHeight="22770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3435" yWindow="14505" windowWidth="23970" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sungau 09-03" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SRO 32-33'!$A$4:$X$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SRO 41'!$A$4:$X$163</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SRO 42'!$A$4:$X$161</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sungau 09-03'!$A$4:$X$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sungau 09-03'!$A$4:$Y$140</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="374">
   <si>
     <t>polesite</t>
   </si>
@@ -1006,9 +1006,6 @@
     <t>COURTAVON</t>
   </si>
   <si>
-    <t>RUE DES CHAUDRONS, LIEBSDORF</t>
-  </si>
-  <si>
     <t>LIEBSDORF</t>
   </si>
   <si>
@@ -1024,9 +1021,6 @@
     <t>68363/39812</t>
   </si>
   <si>
-    <t>RUE DU VIGNOBLE, WERENTZHOUSE</t>
-  </si>
-  <si>
     <t>WERENTZHOUSE</t>
   </si>
   <si>
@@ -1039,9 +1033,6 @@
     <t>68181/141826</t>
   </si>
   <si>
-    <t>RUE D'OBERLAG, LEVONCOURT</t>
-  </si>
-  <si>
     <t>LEVONCOURT</t>
   </si>
   <si>
@@ -1054,27 +1045,18 @@
     <t>BENDORF</t>
   </si>
   <si>
-    <t>Rue Du Pont, BENDORF</t>
-  </si>
-  <si>
     <t>FR8</t>
   </si>
   <si>
     <t>68025/39260</t>
   </si>
   <si>
-    <t>Rue De Ferrette, BENDORF</t>
-  </si>
-  <si>
     <t>FR7</t>
   </si>
   <si>
     <t>68025/39276</t>
   </si>
   <si>
-    <t>Rue Du Cimetière, BENDORF</t>
-  </si>
-  <si>
     <t>MS7</t>
   </si>
   <si>
@@ -1087,22 +1069,13 @@
     <t>SONDERSDORF</t>
   </si>
   <si>
-    <t>Rue Des Vignes, SONDERSDORF</t>
-  </si>
-  <si>
     <t>68186/39843</t>
   </si>
   <si>
     <t>LIGSDORF</t>
   </si>
   <si>
-    <t>Rue Principale, LIGSDORF</t>
-  </si>
-  <si>
     <t>68186/39928</t>
-  </si>
-  <si>
-    <t>Rue De La Birgmatte, LIGSDORF</t>
   </si>
   <si>
     <t>MS8</t>
@@ -1114,9 +1087,6 @@
   <si>
     <t>8 HFT S30
 Dépose BOIS+hauban avec forte flèche- pose métal en arrêt</t>
-  </si>
-  <si>
-    <t>11 RUE DE LUTTER, WOLSCHWILLER</t>
   </si>
   <si>
     <t>FR8
@@ -1126,6 +1096,69 @@
   <si>
     <t>BS7
 BS à changer dans Terre</t>
+  </si>
+  <si>
+    <t>2019020101825D4C</t>
+  </si>
+  <si>
+    <t>2019020102514DDA</t>
+  </si>
+  <si>
+    <t>RUE DES CHAUDRONS, 68480 LIEBSDORF</t>
+  </si>
+  <si>
+    <t>2019020102015D74</t>
+  </si>
+  <si>
+    <t>RUE DU VIGNOBLE, 68480 WERENTZHOUSE</t>
+  </si>
+  <si>
+    <t>2019090404602DAD</t>
+  </si>
+  <si>
+    <t>2019090404226D7A</t>
+  </si>
+  <si>
+    <t>RUE D'OBERLAG, 68480 LEVONCOURT</t>
+  </si>
+  <si>
+    <t>Rue De Ferrette, 68480 BENDORF</t>
+  </si>
+  <si>
+    <t>2019020102487D85</t>
+  </si>
+  <si>
+    <t>2019020102247D1C</t>
+  </si>
+  <si>
+    <t>Rue Du Cimetière, 68480 BENDORF</t>
+  </si>
+  <si>
+    <t>2019020101965D60</t>
+  </si>
+  <si>
+    <t>Rue Principale, 68480 LIGSDORF</t>
+  </si>
+  <si>
+    <t>2019020101927D2B</t>
+  </si>
+  <si>
+    <t>Rue De La Birgmatte, 68480 LIGSDORF</t>
+  </si>
+  <si>
+    <t>Rue Des Vignes, 68480 SONDERSDORF</t>
+  </si>
+  <si>
+    <t>Rue Du Pont, 68480 BENDORF</t>
+  </si>
+  <si>
+    <t>11 RUE DE LUTTER, 68480 WOLSCHWILLER</t>
+  </si>
+  <si>
+    <t>2019020102169DAD</t>
+  </si>
+  <si>
+    <t>Couplé</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1163,6 +1196,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1186,7 +1225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1216,6 +1255,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1491,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0D3C3F-37F4-4BD5-B1D9-FA2000659576}">
-  <dimension ref="A1:X140"/>
+  <dimension ref="A1:Y140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,10 +1559,12 @@
     <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.42578125" customWidth="1"/>
     <col min="20" max="20" width="43.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="13.140625" customWidth="1"/>
+    <col min="21" max="22" width="13.140625" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1548,12 +1590,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>74</v>
@@ -1571,12 +1613,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1644,13 +1686,16 @@
         <v>23</v>
       </c>
       <c r="W4" t="s">
+        <v>373</v>
+      </c>
+      <c r="X4" t="s">
         <v>24</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1662,6 +1707,12 @@
       </c>
       <c r="D5" s="5" t="s">
         <v>322</v>
+      </c>
+      <c r="E5">
+        <v>47.461596999999998</v>
+      </c>
+      <c r="F5">
+        <v>7.192177</v>
       </c>
       <c r="G5" t="s">
         <v>72</v>
@@ -1669,7 +1720,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="5"/>
+      <c r="L5" s="17"/>
       <c r="M5" s="5"/>
       <c r="N5" s="9"/>
       <c r="P5" s="5">
@@ -1679,27 +1730,33 @@
         <v>27</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="U5">
         <v>1</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>324</v>
+        <v>355</v>
+      </c>
+      <c r="E6">
+        <v>47.478356599999998</v>
+      </c>
+      <c r="F6">
+        <v>7.2308630000000003</v>
       </c>
       <c r="G6" t="s">
         <v>72</v>
@@ -1707,7 +1764,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="5"/>
+      <c r="L6" t="s">
+        <v>356</v>
+      </c>
       <c r="M6" s="5"/>
       <c r="N6" s="9"/>
       <c r="P6" s="5">
@@ -1717,24 +1776,30 @@
         <v>27</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="W6">
+        <v>326</v>
+      </c>
+      <c r="X6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>331</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>330</v>
+        <v>357</v>
+      </c>
+      <c r="E7">
+        <v>47.518499599999998</v>
+      </c>
+      <c r="F7">
+        <v>7.3583023000000001</v>
       </c>
       <c r="G7" t="s">
         <v>72</v>
@@ -1742,7 +1807,9 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="5"/>
+      <c r="L7" t="s">
+        <v>358</v>
+      </c>
       <c r="M7" s="5"/>
       <c r="N7" s="9"/>
       <c r="P7" s="5">
@@ -1752,24 +1819,30 @@
         <v>27</v>
       </c>
       <c r="T7" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="W7">
+        <v>349</v>
+      </c>
+      <c r="X7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>360</v>
+        <v>371</v>
+      </c>
+      <c r="E8">
+        <v>47.4625834</v>
+      </c>
+      <c r="F8">
+        <v>7.4048638999999996</v>
       </c>
       <c r="G8" t="s">
         <v>72</v>
@@ -1777,7 +1850,9 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="5"/>
+      <c r="L8" t="s">
+        <v>353</v>
+      </c>
       <c r="M8" s="5"/>
       <c r="N8" s="9"/>
       <c r="P8" s="5">
@@ -1787,24 +1862,30 @@
         <v>125</v>
       </c>
       <c r="T8" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="W8">
+        <v>350</v>
+      </c>
+      <c r="X8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>335</v>
+        <v>360</v>
+      </c>
+      <c r="E9">
+        <v>47.451599000000002</v>
+      </c>
+      <c r="F9">
+        <v>7.2048160000000001</v>
       </c>
       <c r="G9" t="s">
         <v>72</v>
@@ -1812,7 +1893,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="5"/>
+      <c r="L9" t="s">
+        <v>359</v>
+      </c>
       <c r="M9" s="5"/>
       <c r="N9" s="9"/>
       <c r="P9" s="5">
@@ -1822,27 +1905,33 @@
         <v>27</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="U9">
         <v>1</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>340</v>
+        <v>370</v>
+      </c>
+      <c r="E10">
+        <v>47.486294299999997</v>
+      </c>
+      <c r="F10">
+        <v>7.2815817000000003</v>
       </c>
       <c r="G10" t="s">
         <v>72</v>
@@ -1850,7 +1939,9 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="5"/>
+      <c r="L10" t="s">
+        <v>372</v>
+      </c>
       <c r="M10" s="5"/>
       <c r="N10" s="9"/>
       <c r="P10" s="5">
@@ -1860,24 +1951,30 @@
         <v>27</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="W10">
+        <v>337</v>
+      </c>
+      <c r="X10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>343</v>
+        <v>361</v>
+      </c>
+      <c r="E11">
+        <v>47.4883162</v>
+      </c>
+      <c r="F11">
+        <v>7.2830472000000004</v>
       </c>
       <c r="G11" t="s">
         <v>72</v>
@@ -1885,7 +1982,9 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="5"/>
+      <c r="L11" t="s">
+        <v>362</v>
+      </c>
       <c r="M11" s="5"/>
       <c r="N11" s="9"/>
       <c r="P11" s="5">
@@ -1895,24 +1994,30 @@
         <v>27</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="W11">
+        <v>339</v>
+      </c>
+      <c r="X11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>346</v>
+        <v>364</v>
+      </c>
+      <c r="E12">
+        <v>47.487713300000003</v>
+      </c>
+      <c r="F12">
+        <v>7.2789051000000002</v>
       </c>
       <c r="G12" t="s">
         <v>72</v>
@@ -1920,7 +2025,9 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="5"/>
+      <c r="L12" t="s">
+        <v>363</v>
+      </c>
       <c r="M12" s="5"/>
       <c r="N12" s="9"/>
       <c r="P12" s="5">
@@ -1930,27 +2037,33 @@
         <v>27</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="U12">
         <v>1</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>346</v>
+        <v>364</v>
+      </c>
+      <c r="E13">
+        <v>47.487963300000004</v>
+      </c>
+      <c r="F13">
+        <v>7.2791551000000005</v>
       </c>
       <c r="G13" t="s">
         <v>72</v>
@@ -1958,7 +2071,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="5"/>
+      <c r="L13" t="s">
+        <v>363</v>
+      </c>
       <c r="M13" s="5"/>
       <c r="N13" s="9"/>
       <c r="P13" s="5">
@@ -1968,24 +2083,30 @@
         <v>27</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="W13">
+        <v>337</v>
+      </c>
+      <c r="X13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>351</v>
+        <v>369</v>
+      </c>
+      <c r="E14">
+        <v>47.483603700000003</v>
+      </c>
+      <c r="F14">
+        <v>7.3353199</v>
       </c>
       <c r="G14" t="s">
         <v>72</v>
@@ -1993,7 +2114,9 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="5"/>
+      <c r="L14" s="10" t="s">
+        <v>354</v>
+      </c>
       <c r="M14" s="5"/>
       <c r="N14" s="9"/>
       <c r="P14" s="5">
@@ -2003,24 +2126,30 @@
         <v>27</v>
       </c>
       <c r="T14" s="15" t="s">
-        <v>362</v>
-      </c>
-      <c r="W14">
+        <v>352</v>
+      </c>
+      <c r="X14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>354</v>
+        <v>366</v>
+      </c>
+      <c r="E15">
+        <v>47.472806599999998</v>
+      </c>
+      <c r="F15">
+        <v>7.3048944000000002</v>
       </c>
       <c r="G15" t="s">
         <v>72</v>
@@ -2028,7 +2157,9 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="5"/>
+      <c r="L15" t="s">
+        <v>365</v>
+      </c>
       <c r="M15" s="5"/>
       <c r="N15" s="9"/>
       <c r="P15" s="5">
@@ -2038,24 +2169,30 @@
         <v>27</v>
       </c>
       <c r="T15" s="15" t="s">
-        <v>361</v>
-      </c>
-      <c r="W15">
+        <v>351</v>
+      </c>
+      <c r="X15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>356</v>
+        <v>368</v>
+      </c>
+      <c r="E16">
+        <v>47.4714344</v>
+      </c>
+      <c r="F16">
+        <v>7.3098961999999998</v>
       </c>
       <c r="G16" t="s">
         <v>72</v>
@@ -2063,7 +2200,9 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>367</v>
+      </c>
       <c r="M16" s="5"/>
       <c r="N16" s="9"/>
       <c r="P16" s="5">
@@ -2073,16 +2212,13 @@
         <v>27</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="W16">
+        <v>348</v>
+      </c>
+      <c r="X16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2095,10 +2231,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2111,10 +2244,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2127,10 +2257,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -2143,10 +2270,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2159,10 +2283,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>9</v>
-      </c>
+    <row r="22" spans="2:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2177,352 +2298,254 @@
       <c r="Q22" s="11"/>
       <c r="R22" s="13"/>
       <c r="T22" s="14"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
+      <c r="W22"/>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="N23" s="9"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="N24" s="9"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="N25" s="9"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="N26" s="9"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>9</v>
-      </c>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="N27" s="9"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>9</v>
-      </c>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="N28" s="9"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="N29" s="9"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>9</v>
-      </c>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="N30" s="9"/>
-      <c r="W30" s="10"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>9</v>
-      </c>
+      <c r="X30" s="10"/>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="N31" s="9"/>
-      <c r="W31" s="10"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>9</v>
-      </c>
+      <c r="X31" s="10"/>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="N32" s="9"/>
       <c r="T32" s="2"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>9</v>
-      </c>
+    <row r="33" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="N33" s="9"/>
       <c r="T33" s="2"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>9</v>
-      </c>
+    <row r="34" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="N34" s="9"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>9</v>
-      </c>
+    <row r="35" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="N35" s="9"/>
       <c r="T35" s="2"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
+    <row r="36" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="N36" s="9"/>
-      <c r="W36" s="10"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>9</v>
-      </c>
+      <c r="X36" s="10"/>
+    </row>
+    <row r="37" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="N37" s="9"/>
-      <c r="W37" s="10"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>9</v>
-      </c>
+      <c r="X37" s="10"/>
+    </row>
+    <row r="38" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="N38" s="9"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>9</v>
-      </c>
+    <row r="39" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="N39" s="9"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>9</v>
-      </c>
+    <row r="40" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="N40" s="9"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
+    <row r="41" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="N41" s="9"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
+    <row r="42" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="N42" s="9"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>9</v>
-      </c>
+    <row r="43" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="N43" s="9"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>9</v>
-      </c>
+    <row r="44" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="N44" s="9"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>9</v>
-      </c>
+    <row r="45" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="N45" s="9"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>9</v>
-      </c>
+    <row r="46" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="N46" s="9"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>9</v>
-      </c>
+    <row r="47" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="N47" s="9"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>9</v>
-      </c>
+    <row r="48" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="N48" s="9"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>9</v>
-      </c>
+    <row r="49" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="T49" s="2"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>9</v>
-      </c>
+    <row r="50" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="W50" s="10"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>9</v>
-      </c>
+      <c r="X50" s="10"/>
+    </row>
+    <row r="51" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
-      <c r="W51" s="10"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>9</v>
-      </c>
+      <c r="X51" s="10"/>
+    </row>
+    <row r="52" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
-      <c r="W52" s="10"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>9</v>
-      </c>
+      <c r="X52" s="10"/>
+    </row>
+    <row r="53" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
-      <c r="W53" s="10"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>9</v>
-      </c>
+      <c r="X53" s="10"/>
+    </row>
+    <row r="54" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
-      <c r="W54" s="10"/>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>9</v>
-      </c>
+      <c r="X54" s="10"/>
+    </row>
+    <row r="55" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
-      <c r="W55" s="10"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X55" s="10"/>
+    </row>
+    <row r="56" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:24" x14ac:dyDescent="0.25">
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -2908,7 +2931,7 @@
       <c r="K140" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:X140" xr:uid="{79417DF6-A9CB-401D-9FF0-0FB9B9388E9C}"/>
+  <autoFilter ref="A4:Y140" xr:uid="{79417DF6-A9CB-401D-9FF0-0FB9B9388E9C}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
BE+FE RipSites Team Average Stats Refactoring (WIP)
</commit_message>
<xml_diff>
--- a/website/backend/model/polesites/test/Alsace Bonnet Sungau 09-03.xlsx
+++ b/website/backend/model/polesites/test/Alsace Bonnet Sungau 09-03.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DE152F-12F0-4508-903C-DC2C8B30F375}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE077D7C-1F0B-4F25-934C-0853DD58AF28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="14505" windowWidth="23970" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="11235" windowWidth="30435" windowHeight="16485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sungau 09-03" sheetId="6" r:id="rId1"/>
-    <sheet name="SRO 32-33" sheetId="5" r:id="rId2"/>
-    <sheet name="SRO 42" sheetId="4" r:id="rId3"/>
-    <sheet name="SRO 41" sheetId="1" r:id="rId4"/>
-    <sheet name="Dico" sheetId="2" r:id="rId5"/>
+    <sheet name="cernay 09-16" sheetId="7" r:id="rId1"/>
+    <sheet name="Sungau 09-03" sheetId="6" r:id="rId2"/>
+    <sheet name="SRO 32-33" sheetId="5" r:id="rId3"/>
+    <sheet name="SRO 42" sheetId="4" r:id="rId4"/>
+    <sheet name="SRO 41" sheetId="1" r:id="rId5"/>
+    <sheet name="Dico" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SRO 32-33'!$A$4:$X$161</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SRO 41'!$A$4:$X$163</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SRO 42'!$A$4:$X$161</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sungau 09-03'!$A$4:$Y$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SRO 32-33'!$A$4:$X$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'SRO 41'!$A$4:$X$163</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SRO 42'!$A$4:$X$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sungau 09-03'!$A$4:$Y$140</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="388">
   <si>
     <t>polesite</t>
   </si>
@@ -1159,6 +1160,48 @@
   </si>
   <si>
     <t>Couplé</t>
+  </si>
+  <si>
+    <t>Cernay</t>
+  </si>
+  <si>
+    <t>68063/57940</t>
+  </si>
+  <si>
+    <t>Avenue Charles De Gaulle</t>
+  </si>
+  <si>
+    <t>BS8</t>
+  </si>
+  <si>
+    <t>68063/57840</t>
+  </si>
+  <si>
+    <t>41, Avenue Charles De Gaulle</t>
+  </si>
+  <si>
+    <t>68063/57764</t>
+  </si>
+  <si>
+    <t>17 Rue de Graffenwald</t>
+  </si>
+  <si>
+    <t>MF8</t>
+  </si>
+  <si>
+    <t>68063/56690</t>
+  </si>
+  <si>
+    <t>Rue Sandoz</t>
+  </si>
+  <si>
+    <t>68063/57762</t>
+  </si>
+  <si>
+    <t>2 Rue des Pins</t>
+  </si>
+  <si>
+    <t>MI7</t>
   </si>
 </sst>
 </file>
@@ -1530,11 +1573,340 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE308B2D-A67B-423B-A9B8-539728E67302}">
+  <dimension ref="A1:Y9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43724</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" t="s">
+        <v>23</v>
+      </c>
+      <c r="W4" t="s">
+        <v>373</v>
+      </c>
+      <c r="X4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5" t="s">
+        <v>376</v>
+      </c>
+      <c r="E5">
+        <v>47.792383000000001</v>
+      </c>
+      <c r="F5">
+        <v>7.1909640000000001</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P5">
+        <v>8</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" t="s">
+        <v>377</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>378</v>
+      </c>
+      <c r="C6" t="s">
+        <v>374</v>
+      </c>
+      <c r="D6" t="s">
+        <v>379</v>
+      </c>
+      <c r="E6">
+        <v>47.800466</v>
+      </c>
+      <c r="F6">
+        <v>7.182588</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P6">
+        <v>8</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>125</v>
+      </c>
+      <c r="T6" t="s">
+        <v>348</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C7" t="s">
+        <v>374</v>
+      </c>
+      <c r="D7" t="s">
+        <v>381</v>
+      </c>
+      <c r="E7">
+        <v>47.801057999999998</v>
+      </c>
+      <c r="F7">
+        <v>7.1875730000000004</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+      <c r="P7">
+        <v>8</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T7" t="s">
+        <v>382</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" t="s">
+        <v>384</v>
+      </c>
+      <c r="E8">
+        <v>47.807909000000002</v>
+      </c>
+      <c r="F8">
+        <v>7.1554589999999996</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P8">
+        <v>8</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" t="s">
+        <v>377</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>385</v>
+      </c>
+      <c r="C9" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" t="s">
+        <v>386</v>
+      </c>
+      <c r="E9">
+        <v>47.802303000000002</v>
+      </c>
+      <c r="F9">
+        <v>7.18689</v>
+      </c>
+      <c r="G9" t="s">
+        <v>72</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>125</v>
+      </c>
+      <c r="T9" t="s">
+        <v>387</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0D3C3F-37F4-4BD5-B1D9-FA2000659576}">
   <dimension ref="A1:Y140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,7 +3310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F045F09-C25C-45E8-85BF-72D6750066C9}">
   <dimension ref="A1:X161"/>
   <sheetViews>
@@ -6350,7 +6722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB26E745-07E3-4ACD-A5E4-AE3CF8C9BF4F}">
   <dimension ref="A1:X161"/>
   <sheetViews>
@@ -8242,7 +8614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X163"/>
   <sheetViews>
@@ -9807,7 +10179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0499BF6E-E460-42C7-AA22-CE5C456BA101}">
   <dimension ref="A1:A9"/>
   <sheetViews>

</xml_diff>